<commit_message>
working on base billings
</commit_message>
<xml_diff>
--- a/docs/Model_visual.xlsx
+++ b/docs/Model_visual.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidsmith/Documents/Adobe/Deferred_Revenue_Forecast/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A067CB90-4A02-9C42-8DDD-87BA2FAF4347}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15E19BCA-5B90-1C4A-8E75-1CA2E9759D37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{BC15D03B-8830-F841-980F-A95D9CC47D47}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
   <si>
     <t>Tracking Values in Deferred Revenue</t>
   </si>
@@ -144,6 +145,45 @@
   </si>
   <si>
     <t>df_a_1Y</t>
+  </si>
+  <si>
+    <t>df_a_2Y</t>
+  </si>
+  <si>
+    <t>df_a_3Y</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>grouped</t>
+  </si>
+  <si>
+    <t>G2</t>
+  </si>
+  <si>
+    <t>ZCCR</t>
+  </si>
+  <si>
+    <t>ZCDR</t>
+  </si>
+  <si>
+    <t>ZCPR</t>
+  </si>
+  <si>
+    <t>ZLCR</t>
+  </si>
+  <si>
+    <t>ZLDR</t>
+  </si>
+  <si>
+    <t>ZLG2</t>
+  </si>
+  <si>
+    <t>ZRG2</t>
+  </si>
+  <si>
+    <t>ZRL2</t>
   </si>
 </sst>
 </file>
@@ -1043,8 +1083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7147841-957D-6C47-AC9B-1D05A0C45F2B}">
   <dimension ref="B2:AA24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="AA12" sqref="AA12"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1115,6 +1155,12 @@
       </c>
     </row>
     <row r="6" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="I6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="N6" s="20" t="s">
         <v>27</v>
       </c>
@@ -1151,6 +1197,13 @@
       <c r="H7" s="10" t="s">
         <v>11</v>
       </c>
+      <c r="I7" s="1">
+        <f>F8</f>
+        <v>12299</v>
+      </c>
+      <c r="J7" s="1">
+        <v>1403</v>
+      </c>
       <c r="N7" s="20" t="s">
         <v>28</v>
       </c>
@@ -1208,6 +1261,12 @@
       <c r="H9" s="9" t="s">
         <v>12</v>
       </c>
+      <c r="I9" s="1">
+        <v>3058</v>
+      </c>
+      <c r="J9" s="1">
+        <v>581</v>
+      </c>
       <c r="N9" s="14" t="s">
         <v>30</v>
       </c>
@@ -1264,11 +1323,11 @@
         <v>36</v>
       </c>
       <c r="Z11" s="1">
-        <v>906</v>
+        <v>1833</v>
       </c>
       <c r="AA11" s="1">
         <f>AA6-Z11</f>
-        <v>1514</v>
+        <v>587</v>
       </c>
     </row>
     <row r="12" spans="2:27" x14ac:dyDescent="0.2">
@@ -1352,11 +1411,108 @@
         <v>75564</v>
       </c>
     </row>
-    <row r="24" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="Y16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z16" s="1">
+        <v>485</v>
+      </c>
+      <c r="AA16" s="1">
+        <f>AA11-Z16</f>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="10:27" x14ac:dyDescent="0.2">
+      <c r="Y20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z20" s="1">
+        <v>102</v>
+      </c>
+      <c r="AA20" s="1">
+        <f>AA16-Z20</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="10:27" x14ac:dyDescent="0.2">
+      <c r="Y23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z23" s="1">
+        <f>SUM(Z5:Z21)</f>
+        <v>2605</v>
+      </c>
+      <c r="AA23" s="1">
+        <f>AA20</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="10:27" x14ac:dyDescent="0.2">
       <c r="J24" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37D787BF-9E2B-DA4C-B688-C16630C4666C}">
+  <dimension ref="E11:E19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="11" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>